<commit_message>
add construct binary tree from preorder and inorder in the review list
</commit_message>
<xml_diff>
--- a/review_list.xlsx
+++ b/review_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\#project\Algorithm_Questions_Aries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26484817-B8CD-42D6-9095-52F30B044CE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D184581-A6F8-4A48-AA85-0EC0A7DB25A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -176,6 +176,10 @@
   </si>
   <si>
     <t>160. Intersection of Two Linked Lists</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Construct Binary Tree from Preorder and Inorder Traversal</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -501,16 +505,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -695,6 +699,17 @@
       </c>
       <c r="C15" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -709,7 +724,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>